<commit_message>
change the way to show result in excel and compare the result in test
</commit_message>
<xml_diff>
--- a/OrangeHRM/bin/Debug/TestCaseData_Tuong.xlsx
+++ b/OrangeHRM/bin/Debug/TestCaseData_Tuong.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tuongmt\OneDrive\Tài liệu\Huflit\SQualityAssurance\LT\Selenium\OrangeHRM\bin\Debug\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7404F05D-23FB-4CCF-9B9B-F772B729F11D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A0974105-F2AC-44B4-9E84-C2547EC11259}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="870" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="870" firstSheet="2" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ValidUser" sheetId="1" r:id="rId1"/>
@@ -22,18 +22,31 @@
     <sheet name="DeleteCandidate" sheetId="8" r:id="rId7"/>
     <sheet name="EditVacancy" sheetId="9" r:id="rId8"/>
     <sheet name="ViewCandidate" sheetId="10" r:id="rId9"/>
+    <sheet name="ChangeProfilePicture" sheetId="11" r:id="rId10"/>
+    <sheet name="EditPersonalDetails" sheetId="12" r:id="rId11"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="164" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="250" uniqueCount="80">
   <si>
     <t>username</t>
   </si>
@@ -47,142 +60,241 @@
     <t>actual</t>
   </si>
   <si>
+    <t>result</t>
+  </si>
+  <si>
     <t>tuongma</t>
   </si>
   <si>
     <t>Tuong*123</t>
   </si>
   <si>
+    <t>Redirect to Dashboard page</t>
+  </si>
+  <si>
+    <t>Tuong*124</t>
+  </si>
+  <si>
+    <t>Invalid credentials</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t>Required</t>
+  </si>
+  <si>
+    <t>tuong</t>
+  </si>
+  <si>
+    <t>It's valid credentials</t>
+  </si>
+  <si>
+    <t>jobTitle</t>
+  </si>
+  <si>
+    <t>Spokesperson</t>
+  </si>
+  <si>
+    <t>Job Title Name Already exists</t>
+  </si>
+  <si>
+    <t>Manager</t>
+  </si>
+  <si>
+    <t>Job Title Name Required</t>
+  </si>
+  <si>
+    <t>vacancyName</t>
+  </si>
+  <si>
+    <t>hiringManager</t>
+  </si>
+  <si>
+    <t>Tester1</t>
+  </si>
+  <si>
+    <t>Software developer</t>
+  </si>
+  <si>
+    <t>Tuong  Ma</t>
+  </si>
+  <si>
+    <t>Return to Vacancies page when adding success</t>
+  </si>
+  <si>
+    <t>Do not return to Vacancies page when adding success</t>
+  </si>
+  <si>
+    <t>Vacancy Name Already exists</t>
+  </si>
+  <si>
+    <t>Tester2</t>
+  </si>
+  <si>
+    <t>Doctor</t>
+  </si>
+  <si>
+    <t>Job Title isn't exist</t>
+  </si>
+  <si>
+    <t>Tester3</t>
+  </si>
+  <si>
+    <t>Thuyen</t>
+  </si>
+  <si>
+    <t>Hiring Manager is Invalid</t>
+  </si>
+  <si>
+    <t>Vacancy Name Required</t>
+  </si>
+  <si>
+    <t>Tester4</t>
+  </si>
+  <si>
+    <t>Tester5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   </t>
+  </si>
+  <si>
+    <t>Tester6</t>
+  </si>
+  <si>
+    <t>vacancyNo</t>
+  </si>
+  <si>
+    <t>Vacancy is not found</t>
+  </si>
+  <si>
+    <t>Return to Vacancies page when deleting successfully</t>
+  </si>
+  <si>
+    <t>firstName</t>
+  </si>
+  <si>
+    <t>middleName</t>
+  </si>
+  <si>
+    <t>lastName</t>
+  </si>
+  <si>
+    <t>vacancy</t>
+  </si>
+  <si>
+    <t>email</t>
+  </si>
+  <si>
+    <t>Tuong</t>
+  </si>
+  <si>
+    <t>Tuan</t>
+  </si>
+  <si>
+    <t>Ma</t>
+  </si>
+  <si>
+    <t>Tester</t>
+  </si>
+  <si>
+    <t>tuantuong326@gmail.com</t>
+  </si>
+  <si>
     <t>Pass</t>
   </si>
   <si>
-    <t>Fail (Invalid credentials)</t>
-  </si>
-  <si>
-    <t>Tuong*124</t>
-  </si>
-  <si>
-    <t>Fail</t>
-  </si>
-  <si>
-    <t>tuong</t>
-  </si>
-  <si>
-    <t>Fail (It's valid credentials)</t>
-  </si>
-  <si>
-    <t>jobTitle</t>
-  </si>
-  <si>
-    <t>Database developer</t>
-  </si>
-  <si>
-    <t>Fail (Job Title is exist)</t>
-  </si>
-  <si>
-    <t>Database developer2</t>
-  </si>
-  <si>
-    <t>vacancyName</t>
-  </si>
-  <si>
-    <t>hiringManager</t>
-  </si>
-  <si>
-    <t>Tester5</t>
-  </si>
-  <si>
-    <t>Software developer</t>
-  </si>
-  <si>
-    <t>Tuong  Ma</t>
-  </si>
-  <si>
-    <t>Fail (Vacancy Name is exist)</t>
-  </si>
-  <si>
     <t>Tester0109</t>
   </si>
   <si>
-    <t>Tester6</t>
-  </si>
-  <si>
-    <t>Doctor</t>
-  </si>
-  <si>
-    <t>Fail (Job Title isn't exist)</t>
+    <t>Fail (Vacancy not found)</t>
+  </si>
+  <si>
+    <t>tuantuong326@gmai</t>
+  </si>
+  <si>
+    <t>Fail (Email is invalid format)</t>
+  </si>
+  <si>
+    <t>candidateNo</t>
+  </si>
+  <si>
+    <t>Tan  Duong</t>
   </si>
   <si>
     <t>Tester7</t>
   </si>
   <si>
-    <t>Tan Duong</t>
-  </si>
-  <si>
-    <t>Fail (Hiring Manager isn't exist)</t>
-  </si>
-  <si>
-    <t>vacancyNo</t>
-  </si>
-  <si>
-    <t>Fail (Vacancy No not found)</t>
-  </si>
-  <si>
-    <t>firstName</t>
-  </si>
-  <si>
-    <t>middleName</t>
-  </si>
-  <si>
-    <t>lastName</t>
-  </si>
-  <si>
-    <t>vacancy</t>
-  </si>
-  <si>
-    <t>email</t>
-  </si>
-  <si>
-    <t>Tuong</t>
-  </si>
-  <si>
-    <t>Tuan</t>
-  </si>
-  <si>
-    <t>Ma</t>
-  </si>
-  <si>
-    <t>Tester</t>
-  </si>
-  <si>
-    <t>tuantuong326@gmail.com</t>
-  </si>
-  <si>
-    <t>Fail (Vacancy not found)</t>
-  </si>
-  <si>
-    <t>tuantuong326@gmai</t>
-  </si>
-  <si>
-    <t>Fail (Email is invalid format)</t>
-  </si>
-  <si>
-    <t>candidateNo</t>
-  </si>
-  <si>
-    <t>Fail (Candidate No not found)</t>
-  </si>
-  <si>
-    <t>Tan  Duong</t>
-  </si>
-  <si>
     <t>Tester8</t>
+  </si>
+  <si>
+    <t>path</t>
+  </si>
+  <si>
+    <t>C:\Users\tuongmt\studentCard.jpg</t>
+  </si>
+  <si>
+    <t>employeeId</t>
+  </si>
+  <si>
+    <t>otherId</t>
+  </si>
+  <si>
+    <t>licenseNumber</t>
+  </si>
+  <si>
+    <t>licenseExpiryDate</t>
+  </si>
+  <si>
+    <t>nationality</t>
+  </si>
+  <si>
+    <t>maritalStatus</t>
+  </si>
+  <si>
+    <t>dob</t>
+  </si>
+  <si>
+    <t>gender</t>
+  </si>
+  <si>
+    <t>Tai</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Dep </t>
+  </si>
+  <si>
+    <t>Truong</t>
+  </si>
+  <si>
+    <t>0003</t>
+  </si>
+  <si>
+    <t>0033</t>
+  </si>
+  <si>
+    <t>2024-04-04</t>
+  </si>
+  <si>
+    <t>Vietnamese</t>
+  </si>
+  <si>
+    <t>Single</t>
+  </si>
+  <si>
+    <t>2003-12-25</t>
+  </si>
+  <si>
+    <t>Return to Job Titles page when adding successfully</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd;@"/>
+  </numFmts>
   <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -196,14 +308,6 @@
       <color theme="1"/>
       <name val="Times New Roman"/>
       <family val="1"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color theme="10"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
@@ -221,6 +325,12 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF38455D"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -240,23 +350,24 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="49" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="49" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
-  <cellStyles count="2">
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
+  <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -535,19 +646,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D3"/>
+  <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="2" max="2" width="10" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="20.44140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="27.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -560,33 +671,62 @@
       <c r="D1" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C2" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D2" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E2" t="str">
+        <f>IF(EXACT(C2,D2), "Pass", "Fail")</f>
+        <v>Pass</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>8</v>
       </c>
       <c r="C3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D3" t="s">
         <v>9</v>
       </c>
-      <c r="D3" t="s">
+      <c r="E3" t="str">
+        <f>IF(EXACT(C3,D3), "Pass", "Fail")</f>
+        <v>Fail</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A4" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C4" t="s">
         <v>7</v>
+      </c>
+      <c r="D4" t="s">
+        <v>11</v>
+      </c>
+      <c r="E4" t="str">
+        <f>IF(EXACT(C4,D4), "Pass", "Fail")</f>
+        <v>Fail</v>
       </c>
     </row>
   </sheetData>
@@ -594,17 +734,209 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F0538FAA-1A95-4A67-9E65-9049219346AD}">
-  <dimension ref="A1:D3"/>
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0D853A7C-5815-4459-B495-9A524CAB74C5}">
+  <dimension ref="A1:F3"/>
   <sheetViews>
-    <sheetView zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="8.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.21875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="28.6640625" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A2" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="F2" t="str">
+        <f>IF(EXACT(D2,E2), "Pass", "Fail")</f>
+        <v>Pass</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A3" s="3"/>
+      <c r="B3" s="3"/>
+      <c r="C3" s="2"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{53C1C98B-E934-4B33-A4A7-7DFE7DF1BF23}">
+  <dimension ref="A1:P2"/>
+  <sheetViews>
+    <sheetView topLeftCell="B1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="P2" sqref="P2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="3" width="8.88671875" style="2" customWidth="1"/>
+    <col min="4" max="4" width="11.109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8.88671875" style="2" customWidth="1"/>
+    <col min="6" max="6" width="10.33203125" style="2" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="6.77734375" style="2" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="19.77734375" style="2" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="15.44140625" style="3" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="10.21875" style="2" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="11.33203125" style="2" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="10.33203125" style="9" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="9" style="2" bestFit="1" customWidth="1"/>
+    <col min="14" max="15" width="8.88671875" style="2" customWidth="1"/>
+    <col min="16" max="16" width="8.88671875" customWidth="1"/>
+    <col min="17" max="32" width="8.88671875" style="2" customWidth="1"/>
+    <col min="33" max="16384" width="8.88671875" style="2"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="I1" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="J1" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="K1" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="L1" s="9" t="s">
+        <v>68</v>
+      </c>
+      <c r="M1" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="N1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="O1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="P1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A2" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="F2" s="8" t="s">
+        <v>73</v>
+      </c>
+      <c r="G2" s="8" t="s">
+        <v>74</v>
+      </c>
+      <c r="H2" s="2">
+        <v>3</v>
+      </c>
+      <c r="I2" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="J2" s="4" t="s">
+        <v>76</v>
+      </c>
+      <c r="K2" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="L2" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="M2" s="2">
+        <v>1</v>
+      </c>
+      <c r="P2" t="str">
+        <f>IF(EXACT(N2,O2), "Pass", "Fail")</f>
+        <v>Pass</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F0538FAA-1A95-4A67-9E65-9049219346AD}">
+  <dimension ref="A1:E4"/>
+  <sheetViews>
+    <sheetView zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
+      <selection activeCell="D8" sqref="D8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="2" max="2" width="10" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="17.33203125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -617,30 +949,59 @@
       <c r="D1" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="B2">
         <v>123456</v>
       </c>
       <c r="C2" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="D2" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+        <v>9</v>
+      </c>
+      <c r="E2" t="str">
+        <f>IF(EXACT(C2,D2), "Pass", "Fail")</f>
+        <v>Pass</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>5</v>
+        <v>6</v>
+      </c>
+      <c r="C3" t="s">
+        <v>9</v>
       </c>
       <c r="D3" t="s">
+        <v>13</v>
+      </c>
+      <c r="E3" t="str">
+        <f>IF(EXACT(C3,D3), "Pass", "Fail")</f>
+        <v>Fail</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A4" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C4" t="s">
+        <v>9</v>
+      </c>
+      <c r="D4" t="s">
         <v>11</v>
+      </c>
+      <c r="E4" t="str">
+        <f>IF(EXACT(C4,D4), "Pass", "Fail")</f>
+        <v>Fail</v>
       </c>
     </row>
   </sheetData>
@@ -650,10 +1011,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{86F1CF16-D497-4199-9696-F19E7C9263E8}">
-  <dimension ref="A1:E4"/>
+  <dimension ref="A1:F4"/>
   <sheetViews>
-    <sheetView zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+    <sheetView zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -661,10 +1022,11 @@
     <col min="1" max="1" width="9" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="10" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="22" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="18.44140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="43" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="25.21875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -672,7 +1034,7 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="D1" t="s">
         <v>2</v>
@@ -680,38 +1042,70 @@
       <c r="E1" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C2" t="s">
-        <v>13</v>
+        <v>15</v>
+      </c>
+      <c r="D2" t="s">
+        <v>79</v>
       </c>
       <c r="E2" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+        <v>16</v>
+      </c>
+      <c r="F2" t="str">
+        <f>IF(EXACT(D2,E2), "Pass", "Fail")</f>
+        <v>Fail</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C3" t="s">
-        <v>15</v>
+        <v>6</v>
+      </c>
+      <c r="C3" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="D3" t="s">
+        <v>79</v>
       </c>
       <c r="E3" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A4" s="1"/>
-      <c r="B4" s="1"/>
+        <v>16</v>
+      </c>
+      <c r="F3" t="str">
+        <f>IF(EXACT(D3,E3), "Pass", "Fail")</f>
+        <v>Fail</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A4" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C4" s="10"/>
+      <c r="D4" t="s">
+        <v>79</v>
+      </c>
+      <c r="E4" t="s">
+        <v>18</v>
+      </c>
+      <c r="F4" t="str">
+        <f>IF(EXACT(D4,E4), "Pass", "Fail")</f>
+        <v>Fail</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -720,10 +1114,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DCA3E80F-7DE0-4317-9875-6CC0AD481508}">
-  <dimension ref="A1:G5"/>
+  <dimension ref="A1:H9"/>
   <sheetViews>
-    <sheetView zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
-      <selection sqref="A1:G5"/>
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="G13" sqref="G13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -733,9 +1127,11 @@
     <col min="3" max="3" width="14.5546875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="17.21875" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="40.6640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="46.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -743,13 +1139,13 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="D1" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="E1" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="F1" t="s">
         <v>2</v>
@@ -757,85 +1153,211 @@
       <c r="G1" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C2" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="D2" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="E2" t="s">
-        <v>20</v>
+        <v>23</v>
+      </c>
+      <c r="F2" t="s">
+        <v>24</v>
       </c>
       <c r="G2" t="s">
+        <v>25</v>
+      </c>
+      <c r="H2" t="str">
+        <f>IF(EXACT(F2,G2), "Pass", "Fail")</f>
+        <v>Fail</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A3" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C3" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A3" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C3" t="s">
+      <c r="D3" t="s">
         <v>22</v>
       </c>
-      <c r="D3" t="s">
-        <v>19</v>
-      </c>
       <c r="E3" t="s">
-        <v>20</v>
+        <v>23</v>
+      </c>
+      <c r="F3" t="s">
+        <v>24</v>
       </c>
       <c r="G3" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+        <v>26</v>
+      </c>
+      <c r="H3" t="str">
+        <f>IF(EXACT(F3,G3), "Pass", "Fail")</f>
+        <v>Fail</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C4" t="s">
+        <v>27</v>
+      </c>
+      <c r="D4" t="s">
+        <v>28</v>
+      </c>
+      <c r="E4" t="s">
         <v>23</v>
       </c>
-      <c r="D4" t="s">
+      <c r="F4" t="s">
         <v>24</v>
       </c>
-      <c r="E4" t="s">
-        <v>20</v>
-      </c>
       <c r="G4" t="s">
+        <v>29</v>
+      </c>
+      <c r="H4" t="str">
+        <f t="shared" ref="H4:H7" si="0">IF(EXACT(F4,G4), "Pass", "Fail")</f>
+        <v>Fail</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A5" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C5" t="s">
+        <v>30</v>
+      </c>
+      <c r="D5" t="s">
+        <v>22</v>
+      </c>
+      <c r="E5" t="s">
+        <v>31</v>
+      </c>
+      <c r="F5" t="s">
+        <v>24</v>
+      </c>
+      <c r="G5" t="s">
+        <v>32</v>
+      </c>
+      <c r="H5" t="str">
+        <f t="shared" si="0"/>
+        <v>Fail</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A6" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D6" t="s">
+        <v>22</v>
+      </c>
+      <c r="E6" t="s">
+        <v>23</v>
+      </c>
+      <c r="F6" t="s">
+        <v>24</v>
+      </c>
+      <c r="G6" t="s">
+        <v>33</v>
+      </c>
+      <c r="H6" t="str">
+        <f t="shared" si="0"/>
+        <v>Fail</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A7" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C7" t="s">
+        <v>34</v>
+      </c>
+      <c r="E7" t="s">
+        <v>23</v>
+      </c>
+      <c r="F7" t="s">
+        <v>24</v>
+      </c>
+      <c r="G7" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A5" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C5" t="s">
-        <v>26</v>
-      </c>
-      <c r="D5" t="s">
-        <v>19</v>
-      </c>
-      <c r="E5" t="s">
-        <v>27</v>
-      </c>
-      <c r="G5" t="s">
-        <v>28</v>
+      <c r="H7" t="str">
+        <f t="shared" si="0"/>
+        <v>Fail</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A8" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C8" t="s">
+        <v>35</v>
+      </c>
+      <c r="D8" t="s">
+        <v>36</v>
+      </c>
+      <c r="E8" t="s">
+        <v>23</v>
+      </c>
+      <c r="F8" t="s">
+        <v>24</v>
+      </c>
+      <c r="G8" t="s">
+        <v>29</v>
+      </c>
+      <c r="H8" t="str">
+        <f>IF(EXACT(F9,G8), "Pass", "Fail")</f>
+        <v>Fail</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A9" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C9" t="s">
+        <v>37</v>
+      </c>
+      <c r="D9" t="s">
+        <v>22</v>
+      </c>
+      <c r="F9" t="s">
+        <v>24</v>
+      </c>
+      <c r="G9" t="s">
+        <v>32</v>
       </c>
     </row>
   </sheetData>
@@ -846,10 +1368,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4F03B891-B879-4A0A-BEF2-CA155E95A337}">
-  <dimension ref="A1:E3"/>
+  <dimension ref="A1:F4"/>
   <sheetViews>
-    <sheetView zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+    <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -857,12 +1379,11 @@
     <col min="1" max="1" width="9" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="10" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="12.44140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="17.21875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="44.77734375" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="6.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -870,7 +1391,7 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>29</v>
+        <v>38</v>
       </c>
       <c r="D1" t="s">
         <v>2</v>
@@ -878,33 +1399,68 @@
       <c r="E1" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C2">
-        <v>3</v>
+        <v>6</v>
+      </c>
+      <c r="D2" t="s">
+        <v>40</v>
       </c>
       <c r="E2" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+        <v>39</v>
+      </c>
+      <c r="F2" t="str">
+        <f>IF(EXACT(D2,E2), "Pass", "Fail")</f>
+        <v>Fail</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C3" s="7">
-        <v>333</v>
+        <v>6</v>
+      </c>
+      <c r="C3">
+        <v>1</v>
+      </c>
+      <c r="D3" t="s">
+        <v>40</v>
       </c>
       <c r="E3" t="s">
-        <v>30</v>
+        <v>40</v>
+      </c>
+      <c r="F3" t="str">
+        <f>IF(EXACT(D3,E3), "Pass", "Fail")</f>
+        <v>Pass</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A4" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C4" s="7">
+        <v>1111</v>
+      </c>
+      <c r="D4" t="s">
+        <v>40</v>
+      </c>
+      <c r="E4" t="s">
+        <v>39</v>
+      </c>
+      <c r="F4" t="str">
+        <f>IF(EXACT(D4,E4), "Pass", "Fail")</f>
+        <v>Fail</v>
       </c>
     </row>
   </sheetData>
@@ -914,10 +1470,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2C4AD822-807E-493C-9A4A-D49C23BDC73E}">
-  <dimension ref="A1:I4"/>
+  <dimension ref="A1:J4"/>
   <sheetViews>
     <sheetView zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="H1" sqref="H1:I1"/>
+      <selection activeCell="J1" sqref="J1:J1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -930,7 +1486,7 @@
     <col min="8" max="8" width="6.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -938,19 +1494,19 @@
         <v>1</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>31</v>
+        <v>41</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>32</v>
+        <v>42</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>33</v>
+        <v>43</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>34</v>
+        <v>44</v>
       </c>
       <c r="G1" s="5" t="s">
-        <v>35</v>
+        <v>45</v>
       </c>
       <c r="H1" s="2" t="s">
         <v>2</v>
@@ -958,92 +1514,102 @@
       <c r="I1" s="2" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>36</v>
+        <v>46</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>37</v>
+        <v>47</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>38</v>
+        <v>48</v>
       </c>
       <c r="F2" s="4" t="s">
-        <v>39</v>
-      </c>
-      <c r="G2" s="8" t="s">
-        <v>40</v>
+        <v>49</v>
+      </c>
+      <c r="G2" s="11" t="s">
+        <v>50</v>
       </c>
       <c r="H2" s="2"/>
       <c r="I2" s="2" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+        <v>51</v>
+      </c>
+      <c r="J2" t="str">
+        <f>IF(EXACT(H2,I2), "Pass", "Fail")</f>
+        <v>Fail</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>36</v>
+        <v>46</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>37</v>
+        <v>47</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>38</v>
+        <v>48</v>
       </c>
       <c r="F3" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="G3" s="8" t="s">
-        <v>40</v>
+        <v>52</v>
+      </c>
+      <c r="G3" s="11" t="s">
+        <v>50</v>
       </c>
       <c r="I3" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
+        <v>53</v>
+      </c>
+      <c r="J3" t="str">
+        <f>IF(EXACT(H3,I3), "Pass", "Fail")</f>
+        <v>Fail</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A4" s="3" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>36</v>
+        <v>46</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>37</v>
+        <v>47</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>38</v>
+        <v>48</v>
       </c>
       <c r="F4" s="4" t="s">
-        <v>39</v>
-      </c>
-      <c r="G4" s="8" t="s">
-        <v>42</v>
+        <v>49</v>
+      </c>
+      <c r="G4" s="11" t="s">
+        <v>54</v>
       </c>
       <c r="I4" t="s">
-        <v>43</v>
+        <v>55</v>
+      </c>
+      <c r="J4" t="str">
+        <f>IF(EXACT(H4,I4), "Pass", "Fail")</f>
+        <v>Fail</v>
       </c>
     </row>
   </sheetData>
-  <hyperlinks>
-    <hyperlink ref="G2" r:id="rId1" xr:uid="{00000000-0004-0000-0500-000000000000}"/>
-    <hyperlink ref="G3" r:id="rId2" xr:uid="{00000000-0004-0000-0500-000001000000}"/>
-    <hyperlink ref="G4" r:id="rId3" xr:uid="{00000000-0004-0000-0500-000002000000}"/>
-  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait"/>
 </worksheet>
@@ -1051,10 +1617,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A81815B1-E3AD-453F-AFA8-92B78834875B}">
-  <dimension ref="A1:E3"/>
+  <dimension ref="A1:F3"/>
   <sheetViews>
     <sheetView zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection sqref="A1:E3"/>
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1062,7 +1628,7 @@
     <col min="3" max="3" width="11.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -1070,7 +1636,7 @@
         <v>1</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>44</v>
+        <v>56</v>
       </c>
       <c r="D1" s="2" t="s">
         <v>2</v>
@@ -1078,33 +1644,38 @@
       <c r="E1" s="2" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C2" s="2">
         <v>3</v>
       </c>
-      <c r="E2" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F2" t="str">
+        <f>IF(EXACT(D2,E2), "Pass", "Fail")</f>
+        <v>Pass</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C3" s="2">
         <v>333</v>
       </c>
-      <c r="E3" t="s">
-        <v>45</v>
+      <c r="F3" t="str">
+        <f>IF(EXACT(D3,E3), "Pass", "Fail")</f>
+        <v>Pass</v>
       </c>
     </row>
   </sheetData>
@@ -1114,10 +1685,10 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EDF72E7D-0E60-4A95-BFD3-CC2842621BD5}">
-  <dimension ref="A1:H5"/>
+  <dimension ref="A1:I5"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="220" zoomScaleNormal="220" workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
+    <sheetView zoomScale="220" zoomScaleNormal="220" workbookViewId="0">
+      <selection activeCell="I3" sqref="I3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1127,7 +1698,7 @@
     <col min="6" max="6" width="12.77734375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -1135,16 +1706,16 @@
         <v>1</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>29</v>
+        <v>38</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="G1" s="2" t="s">
         <v>2</v>
@@ -1152,101 +1723,112 @@
       <c r="H1" s="2" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C2" s="2">
         <v>3</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>23</v>
+        <v>37</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="F2" s="4" t="s">
-        <v>46</v>
+        <v>57</v>
       </c>
       <c r="G2" s="2"/>
-      <c r="H2" s="2" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="H2" s="2"/>
+      <c r="I2" t="str">
+        <f>IF(EXACT(G2,H2), "Pass", "Fail")</f>
+        <v>Pass</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C3" s="2">
         <v>1</v>
       </c>
       <c r="D3" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="E3" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="E3" s="2" t="s">
-        <v>19</v>
-      </c>
       <c r="F3" s="4" t="s">
-        <v>46</v>
+        <v>57</v>
       </c>
       <c r="G3" s="2"/>
-      <c r="H3" s="2" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="H3" s="2"/>
+      <c r="I3" t="str">
+        <f>IF(EXACT(G3,H3), "Pass", "Fail")</f>
+        <v>Pass</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A4" s="3" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C4" s="2">
         <v>4</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>26</v>
+        <v>58</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>24</v>
+        <v>28</v>
       </c>
       <c r="F4" s="4" t="s">
-        <v>46</v>
+        <v>57</v>
       </c>
       <c r="G4" s="2"/>
-      <c r="H4" s="2" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="H4" s="2"/>
+      <c r="I4" t="str">
+        <f t="shared" ref="I4:I5" si="0">IF(EXACT(G4,H4), "Pass", "Fail")</f>
+        <v>Pass</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A5" s="3" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C5" s="2">
         <v>2</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>47</v>
+        <v>59</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="F5" s="4" t="s">
-        <v>46</v>
+        <v>57</v>
       </c>
       <c r="G5" s="2"/>
-      <c r="H5" s="2" t="s">
-        <v>6</v>
+      <c r="H5" s="2"/>
+      <c r="I5" t="str">
+        <f t="shared" si="0"/>
+        <v>Pass</v>
       </c>
     </row>
   </sheetData>
@@ -1256,10 +1838,10 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{72633E73-3EA9-4C06-9CC3-C9D6199D7235}">
-  <dimension ref="A1:E3"/>
+  <dimension ref="A1:F3"/>
   <sheetViews>
     <sheetView zoomScale="220" zoomScaleNormal="220" workbookViewId="0">
-      <selection activeCell="E3" sqref="E2:E3"/>
+      <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1270,7 +1852,7 @@
     <col min="5" max="5" width="12.77734375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -1278,7 +1860,7 @@
         <v>1</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>44</v>
+        <v>56</v>
       </c>
       <c r="D1" s="2" t="s">
         <v>2</v>
@@ -1286,33 +1868,38 @@
       <c r="E1" s="2" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C2" s="2">
         <v>3</v>
       </c>
-      <c r="E2" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F2" t="str">
+        <f>IF(EXACT(D2,E2), "Pass", "Fail")</f>
+        <v>Pass</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C3" s="2">
         <v>333</v>
       </c>
-      <c r="E3" t="s">
-        <v>45</v>
+      <c r="F3" t="str">
+        <f>IF(EXACT(D3,E3), "Pass", "Fail")</f>
+        <v>Pass</v>
       </c>
     </row>
   </sheetData>

</xml_diff>